<commit_message>
Update Daily Tasksheet.xlsx & Notes.xlsx #LongDB
</commit_message>
<xml_diff>
--- a/wiki/Notes.xlsx
+++ b/wiki/Notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>File</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Thêm cột AssignedDate (mô tả ngày request được gán)</t>
+  </si>
+  <si>
+    <t>Thêm cột Payment (bit-request đã được thanh toán chưa)</t>
+  </si>
+  <si>
+    <t>Thêm cột RequestCode (nvarchar-code cho staff check để thanh toán)</t>
   </si>
 </sst>
 </file>
@@ -254,14 +260,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,17 +589,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -594,203 +616,219 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5">
+    <row r="2" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="7">
         <v>41717</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
+    <row r="3" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
         <v>41717</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+    <row r="4" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
         <v>41717</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="9"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="9"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="9"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="9"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="9"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="9"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="9"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="9"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="9"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="9"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="9"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="9"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="9"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="9"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="9"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="9"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="2:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="9"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="2:5" s="8" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="10"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
+    <row r="5" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>41717</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>41717</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="10"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="10"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="10"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="10"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="10"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="10"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="10"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="10"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="2:5" s="9" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Team chú ý file này, cần sửa những gì đã note trong đây Ai sửa xong phần nào vô cập nhật nha #LongDB
</commit_message>
<xml_diff>
--- a/wiki/Notes.xlsx
+++ b/wiki/Notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>File</t>
   </si>
@@ -55,6 +55,59 @@
   </si>
   <si>
     <t>Thêm cột RequestCode (nvarchar-code cho staff check để thanh toán)</t>
+  </si>
+  <si>
+    <t>SentRequest</t>
+  </si>
+  <si>
+    <t>Hiển thị khoảng cách hoặc đường đi từ địa chỉ của người gửi đến trạm gần nhất để thuận tiện.</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>_LayoutStaff</t>
+  </si>
+  <si>
+    <t>InputInvoice</t>
+  </si>
+  <si>
+    <t>Trong phần nhập hóa đơn, đưa thông tin về khối lượng và thể tích của khách hàng đã post 
+ở phần request để nhân viên chỉnh sửa lại (chứ không nhập từ đầu).</t>
+  </si>
+  <si>
+    <t>Bỏ google map trên layout của nhân viên 
+(sửa LogOn, Login xong phải direct ra đúng page theo role)</t>
+  </si>
+  <si>
+    <t>InvoicePDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format lại Invoice </t>
+  </si>
+  <si>
+    <t>ListRequest</t>
+  </si>
+  <si>
+    <t>Trong phần chi tiết chuyến đi, bỏ phần “Giờ dự kiến đến” (đến trạm cuối) của xe.</t>
+  </si>
+  <si>
+    <t>Thêm mã request của gói hàng trong các chuyến xe chuyển đi để dễ nhận biết và xử lý.</t>
+  </si>
+  <si>
+    <t>ListTrip</t>
+  </si>
+  <si>
+    <t>ExpiredRequest</t>
+  </si>
+  <si>
+    <t>Khi trả hàng lại thì cần đưa ra 2 lựa chọn là: trả hàng hay là hủy luôn gói hàng đó.</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -99,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -242,11 +295,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -267,22 +365,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,24 +692,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E30"/>
+  <dimension ref="B1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -615,8 +722,11 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7">
         <v>41717</v>
       </c>
@@ -629,8 +739,9 @@
       <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>41717</v>
       </c>
@@ -643,8 +754,9 @@
       <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>41717</v>
       </c>
@@ -657,8 +769,9 @@
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>41717</v>
       </c>
@@ -671,8 +784,9 @@
       <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>41717</v>
       </c>
@@ -685,150 +799,233 @@
       <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>41738</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="2:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>41738</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>41738</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>41738</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>41738</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
+        <v>41738</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>41738</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="9"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="2:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="2:5" s="9" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="6"/>
+      <c r="F30" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>